<commit_message>
Video with audio files Updated
</commit_message>
<xml_diff>
--- a/Content.xlsx
+++ b/Content.xlsx
@@ -443,140 +443,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Why don't scientists trust atoms? Because they make up everything!</t>
+          <t>Did you know that cats can make over 100 different sounds? Dogs, on the other hand, can barely muster a couple of "woofs."</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Did you hear about the mathematician who's afraid of negative numbers? He'll stop at nothing to avoid them.</t>
+          <t>Fact: Penguins are great comedians. Isn't it amazing how they can be so funny without even cracking a smile?</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>I used to be a baker, but I couldn't make enough dough. So, I decided to become a banker instead.</t>
+          <t>Did you know that dolphins are always smiling? It's probably because they know they're the smartest fish in the sea!</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>I asked the librarian if there were any books on paranoia. She whispered, "They're right behind you."</t>
+          <t>Fact: The average American eats around 35 tons of food in their lifetime. But my guess is that half of that is just pizza and ice cream!</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Did you hear about the cross-eyed teacher who lost her job because she couldn't control her pupils?</t>
+          <t>Did you know that frogs are great jumpers? They're basically the Olympic athletes of the amphibian world!</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Why did the scarecrow win an award? Because he was outstanding in his field!</t>
+          <t>Fact: The average person laughs around 13 times a day. Unless, of course, they forget to wear their funny socks—then it drops down to zero!</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>How do you organize a space party? You planet!</t>
+          <t>Did you know that squirrels forget where they bury about half of their nuts? That's why we find them in the most unexpected places!</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Did you hear about the man who fell into an upholstery machine? He's fully recovered now!</t>
+          <t>Fact: It takes an average of 364 licks to get to the center of a Tootsie Pop. But who has the patience for that? Just take a bite!</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Why don't skeletons fight each other? They don't have the guts!</t>
+          <t>Did you know that ducks have feathers to cover their butt quacks? It's true! That way, they can keep their tails wagging with dignity!</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>I went to buy some camo pants, but I couldn't find any.</t>
+          <t>Fact: The world's largest recorded snowflake measured 15 inches in diameter. That must have been a very confused snowman!</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>My wife told me I should do lunges to stay in shape. That would be a big step forward.</t>
+          <t>Did you know that mosquitos are the deadliest animals in the world? They're just trying to tell us to invest in bug spray!</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A friend of mine tried to annoy me with bird puns, but I soon realized that toucan play at that game.</t>
+          <t>Fact: The average person spends around six months of their lifetime waiting at red lights. That's a lot of car karaoke time wasted!</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>What kind of shoes do ninjas wear? Sneakers.</t>
+          <t>Did you know that honey never spoils? So the next time someone makes a bee pun, just tell them that joke will never get old!</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>How does Moses make his coffee? Hebrews it.</t>
+          <t>Fact: Banging your head against a wall for one hour burns 150 calories. But I'm not sure it's the most effective workout routine!</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Did you hear about the cheese factory that exploded in France? There was nothing left but de Brie!</t>
+          <t>Did you know that elephants are the only animals that can't jump? No wonder they're always so grounded and accommodating!</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Why did the stadium get hot after the game? Because all of the fans left.</t>
+          <t>Fact: The average person blinks around 17,000 times a day. That's a lot of missed opportunities to admire cute animals and epic sunsets!</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>What did one wall say to the other wall? I'll meet you at the corner.</t>
+          <t>Did you know that the first oranges weren't actually orange? They were green like limes! Talk about a citrus transformation!</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>I asked the gym instructor if he could teach me to do the splits. He replied, "How flexible are you?" I said, "I can't make it on Mondays."</t>
+          <t>Fact: The slogan "Imagination at Work" was once considered by deodorant brand Axe. Can you imagine? Smelling like a wild adventure!</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Why don't skeletons fight in wars? They don't have the guts!</t>
+          <t>Did you know that cows have best friends? They udderly cherish their companionship, making everyday moosic together!</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>What did the grape say when it got stepped on? Nothing, it just let out a little wine.</t>
+          <t>Fact: The world's largest recorded pizza measured 131 feet in diameter. Imagine the size of the delivery guy's car!</t>
         </is>
       </c>
     </row>

</xml_diff>